<commit_message>
Major updates: 1. Migrasi codebase, kini menggunakan Vuex sebagai state management, 2. Memisahkan konfigurasi ke dalam file tersendiri
</commit_message>
<xml_diff>
--- a/ui/src/assets/docs/FormatDataSiswa.xlsx
+++ b/ui/src/assets/docs/FormatDataSiswa.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\smartscore\public\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp7\htdocs\smartscore\ui\src\assets\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1737,8 +1737,8 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Pembaruan modul kelola siswa: - Menambahkan isian rombel - Menambahkan fitur hapus semua data - Memperbaiki warna teks pada <option> di form siswa
</commit_message>
<xml_diff>
--- a/ui/src/assets/docs/FormatDataSiswa.xlsx
+++ b/ui/src/assets/docs/FormatDataSiswa.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1738,7 +1738,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>41</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -1926,6 +1926,9 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>32</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>40</v>
       </c>
@@ -1970,6 +1973,9 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>30</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>139</v>
       </c>
@@ -2014,6 +2020,9 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>31</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>140</v>
       </c>
@@ -2058,6 +2067,9 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>32</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>141</v>
       </c>
@@ -2102,6 +2114,9 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>30</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>142</v>
       </c>
@@ -2146,6 +2161,9 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>31</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>143</v>
       </c>
@@ -2190,6 +2208,9 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>32</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>144</v>
       </c>
@@ -2234,6 +2255,9 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>30</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>145</v>
       </c>
@@ -2278,6 +2302,9 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>31</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>146</v>
       </c>
@@ -2322,6 +2349,9 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>32</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>147</v>
       </c>
@@ -2366,6 +2396,9 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>30</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>148</v>
       </c>
@@ -2410,6 +2443,9 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>31</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>149</v>
       </c>
@@ -2454,6 +2490,9 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>32</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>150</v>
       </c>
@@ -2497,7 +2536,10 @@
         <v>12345678912</v>
       </c>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>30</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>151</v>
       </c>
@@ -2541,7 +2583,10 @@
         <v>12345678912</v>
       </c>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>31</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>152</v>
       </c>
@@ -2585,7 +2630,10 @@
         <v>12345678913</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>32</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>153</v>
       </c>
@@ -2629,7 +2677,10 @@
         <v>12345678914</v>
       </c>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>30</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>154</v>
       </c>
@@ -2673,7 +2724,10 @@
         <v>12345678915</v>
       </c>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>31</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>155</v>
       </c>
@@ -2717,7 +2771,10 @@
         <v>12345678916</v>
       </c>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>32</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>156</v>
       </c>
@@ -2761,7 +2818,10 @@
         <v>12345678917</v>
       </c>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>30</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>157</v>
       </c>
@@ -2805,7 +2865,10 @@
         <v>12345678918</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>31</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>158</v>
       </c>
@@ -2849,7 +2912,10 @@
         <v>12345678919</v>
       </c>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>32</v>
+      </c>
       <c r="C25" s="1" t="s">
         <v>159</v>
       </c>

</xml_diff>

<commit_message>
- Menambahkan fitur naik tingkat kelas - Nama rombel kini dibuat secara otomatis saat memilih tingkat dan paralel - Menghilangkan fungsi duplikat rombel - Memperbarui menu aplikasi - Memperbarui format impor data siswa - Memperbaiki bug pada pemanggilan pagination di data rombel dan siswa - Menyederhanakan pemanggilan alert setelah menghapus data siswa - Kini menampilkan ID rombel pada daftar rombel - Menghilangkan scroll-to content setelah mengupdate data siswa - Memperbarui .gitignore
</commit_message>
<xml_diff>
--- a/ui/src/assets/docs/FormatDataSiswa.xlsx
+++ b/ui/src/assets/docs/FormatDataSiswa.xlsx
@@ -1737,7 +1737,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5:B25"/>
     </sheetView>
   </sheetViews>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>41</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>40</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>139</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>140</v>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>141</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>142</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>143</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>144</v>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>145</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>146</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>147</v>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>148</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>149</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>150</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>151</v>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>152</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>153</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>154</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>155</v>
@@ -2773,7 +2773,7 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>156</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>157</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>158</v>
@@ -2914,7 +2914,7 @@
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
Melengkapi API access token untuk semua request ke controller.
</commit_message>
<xml_diff>
--- a/ui/src/assets/docs/FormatDataSiswa.xlsx
+++ b/ui/src/assets/docs/FormatDataSiswa.xlsx
@@ -1737,8 +1737,8 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>41</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>40</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>139</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>140</v>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>141</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>142</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>143</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>144</v>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>145</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>146</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>147</v>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>148</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>149</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>150</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>151</v>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>152</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>153</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>154</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>155</v>
@@ -2773,7 +2773,7 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>156</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>157</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>158</v>
@@ -2914,7 +2914,7 @@
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
Update apache, mysql dan PHP
</commit_message>
<xml_diff>
--- a/ui/src/assets/docs/FormatDataSiswa.xlsx
+++ b/ui/src/assets/docs/FormatDataSiswa.xlsx
@@ -1738,7 +1738,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>41</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>40</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>139</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>140</v>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>141</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>142</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>143</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>144</v>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>145</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>146</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>147</v>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>148</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>149</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>150</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>151</v>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>152</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>153</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>154</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>155</v>
@@ -2773,7 +2773,7 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>156</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>157</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>158</v>
@@ -2914,7 +2914,7 @@
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
Mengurangi field/isian data siswa.
</commit_message>
<xml_diff>
--- a/ui/src/assets/docs/FormatDataSiswa.xlsx
+++ b/ui/src/assets/docs/FormatDataSiswa.xlsx
@@ -1737,8 +1737,8 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B25"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>41</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>40</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>139</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>140</v>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>141</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>142</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>143</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>144</v>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>145</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>146</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>147</v>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>148</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>149</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>150</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>151</v>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>152</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>153</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>154</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>155</v>
@@ -2773,7 +2773,7 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>156</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>157</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>158</v>
@@ -2914,7 +2914,7 @@
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>159</v>

</xml_diff>